<commit_message>
logistic regression 2th commit
</commit_message>
<xml_diff>
--- a/excel/logistic_regression.xlsx
+++ b/excel/logistic_regression.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspaces\studyAI\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29DD38C2-0D49-46D1-8E65-29C8BC4504DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C4370C6-D35F-467F-96BB-FC2361B2C765}"/>
+    <workbookView xWindow="-240" yWindow="60" windowWidth="25600" windowHeight="14900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>theta(5,)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,16 +42,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H_theta_x(6,)
-X dot theta</t>
+    <t>H_theta_x(6,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X dot theta(6,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temp1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temp2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X^T(5,6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H-theta_x-y(6,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X^T dot (H-theta_x-y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gradient</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,8 +107,34 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,6 +153,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -109,12 +175,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -127,9 +223,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -187,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -239,7 +351,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -433,63 +545,85 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B2205D-92D0-49E9-A9D0-C2CA181848C1}">
-  <dimension ref="B8:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B8:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="8" spans="2:21">
+      <c r="B8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="P8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U8" s="4">
+        <f>AVERAGE(U9:U14)</f>
+        <v>0.69314718055994484</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
         <v>10</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>11</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>12</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>13</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>14</v>
       </c>
       <c r="K9" s="2">
@@ -499,24 +633,40 @@
         <f>E9*$C$9+F9*$C$10+G9*$C$11+H9*$C$12+I9*$C$13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="O9">
+        <f>1/(1+EXP(-M9))</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q9">
+        <f>-1*(K9*LN(O9))</f>
+        <v>69.314718055994533</v>
+      </c>
+      <c r="S9">
+        <f>(1-K9)*LN(1-O9)</f>
+        <v>68.621570875434585</v>
+      </c>
+      <c r="U9">
+        <f>Q9-S9</f>
+        <v>0.69314718055994717</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
         <v>20</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>21</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>22</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>23</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>24</v>
       </c>
       <c r="K10" s="2">
@@ -526,24 +676,40 @@
         <f t="shared" ref="M10:M14" si="0">E10*$C$9+F10*$C$10+G10*$C$11+H10*$C$12+I10*$C$13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="O10">
+        <f t="shared" ref="O10:O14" si="1">1/(1+EXP(-M10))</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10:Q14" si="2">-1*(K10*LN(O10))</f>
+        <v>70.00786523655448</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ref="S10:S14" si="3">(1-K10)*LN(1-O10)</f>
+        <v>69.314718055994533</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ref="U10:U14" si="4">Q10-S10</f>
+        <v>0.69314718055994717</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
         <v>30</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>31</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>32</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>33</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>34</v>
       </c>
       <c r="K11" s="2">
@@ -553,24 +719,40 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>70.701012417114413</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>70.00786523655448</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="4"/>
+        <v>0.69314718055993296</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
         <v>40</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>41</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>42</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>43</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>44</v>
       </c>
       <c r="K12" s="2">
@@ -580,24 +762,40 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>71.39415959767436</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>70.701012417114413</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="4"/>
+        <v>0.69314718055994717</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
         <v>50</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>51</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>52</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>53</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>54</v>
       </c>
       <c r="K13" s="2">
@@ -607,21 +805,37 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="E14">
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>72.087306778234307</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>71.39415959767436</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="4"/>
+        <v>0.69314718055994717</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="E14" s="2">
         <v>60</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>61</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>62</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>63</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>64</v>
       </c>
       <c r="K14" s="2">
@@ -630,11 +844,212 @@
       <c r="M14">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>72.780453958794254</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>72.087306778234307</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="4"/>
+        <v>0.69314718055994717</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17">
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <v>40</v>
+      </c>
+      <c r="I17">
+        <v>50</v>
+      </c>
+      <c r="J17">
+        <v>60</v>
+      </c>
+      <c r="M17">
+        <f>O9-K9</f>
+        <v>-99.5</v>
+      </c>
+      <c r="O17">
+        <f>E17*$M$17+F17*$M$18+G17*$M$19+H17*$M$20+I17*$M$21+J17*$M$22</f>
+        <v>-21595</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>O17*(1/6)</f>
+        <v>-3599.1666666666665</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17">
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>21</v>
+      </c>
+      <c r="G18">
+        <v>31</v>
+      </c>
+      <c r="H18">
+        <v>41</v>
+      </c>
+      <c r="I18">
+        <v>51</v>
+      </c>
+      <c r="J18">
+        <v>61</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M22" si="5">O10-K10</f>
+        <v>-100.5</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O22" si="6">E18*$M$17+F18*$M$18+G18*$M$19+H18*$M$20+I18*$M$21+J18*$M$22</f>
+        <v>-22207</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" ref="Q18:Q21" si="7">O18*(1/6)</f>
+        <v>-3701.1666666666665</v>
+      </c>
+    </row>
+    <row r="19" spans="5:17">
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>22</v>
+      </c>
+      <c r="G19">
+        <v>32</v>
+      </c>
+      <c r="H19">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <v>52</v>
+      </c>
+      <c r="J19">
+        <v>62</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="5"/>
+        <v>-101.5</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>-22819</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="7"/>
+        <v>-3803.1666666666665</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17">
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>33</v>
+      </c>
+      <c r="H20">
+        <v>43</v>
+      </c>
+      <c r="I20">
+        <v>53</v>
+      </c>
+      <c r="J20">
+        <v>63</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="5"/>
+        <v>-102.5</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>-23431</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="7"/>
+        <v>-3905.1666666666665</v>
+      </c>
+    </row>
+    <row r="21" spans="5:17">
+      <c r="E21">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>24</v>
+      </c>
+      <c r="G21">
+        <v>34</v>
+      </c>
+      <c r="H21">
+        <v>44</v>
+      </c>
+      <c r="I21">
+        <v>54</v>
+      </c>
+      <c r="J21">
+        <v>64</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="5"/>
+        <v>-103.5</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>-24043</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="7"/>
+        <v>-4007.1666666666665</v>
+      </c>
+    </row>
+    <row r="22" spans="5:17">
+      <c r="M22">
+        <f t="shared" si="5"/>
+        <v>-104.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>